<commit_message>
update registers to give the trigger core space
</commit_message>
<xml_diff>
--- a/helix_mtrig_registers.xlsx
+++ b/helix_mtrig_registers.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="97">
   <si>
     <t>Master trigger register map, as of 0.1.3</t>
   </si>
@@ -69,12 +69,6 @@
   </si>
   <si>
     <t>Number of 80 MHz clock cycles that trigger is held off</t>
-  </si>
-  <si>
-    <t>SOFTTRIG</t>
-  </si>
-  <si>
-    <t>write 1 to this register to generate soft trig (if enabled). Does not require UPDATE.</t>
   </si>
   <si>
     <t>RANDTRIG</t>
@@ -326,6 +320,24 @@
   </si>
   <si>
     <t>[6] SOFTTRIG, [5] RANDTRIG, [4] PPSTRIG, [3] ZHI, [2] ZLO, [1] EXT, [0] TRIGEN. [15:8] = number of clock cycles to hold off enabling trigger after UPDATE.</t>
+  </si>
+  <si>
+    <t>CPUCONTROL</t>
+  </si>
+  <si>
+    <t>Bit[15]: CPU inhibit mode (at UPDATE). Write 1 to this register to generate soft trig (if enabled). Does not require UPDATE. Write 2 to this register to clear CPUINHIBIT. Does not require UPDATE.</t>
+  </si>
+  <si>
+    <t>BUSYCTRL</t>
+  </si>
+  <si>
+    <t>RSTCTRL</t>
+  </si>
+  <si>
+    <t>[5:0] issue a pulse on FST_CTRL</t>
+  </si>
+  <si>
+    <t>[13:8] current busies, [5:0] busy mask</t>
   </si>
 </sst>
 </file>
@@ -661,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C59"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -740,7 +752,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -759,10 +771,10 @@
         <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>15</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -770,10 +782,10 @@
         <v>7</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -781,10 +793,10 @@
         <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
         <v>19</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -792,10 +804,10 @@
         <v>9</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
         <v>20</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -803,10 +815,10 @@
         <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -814,10 +826,10 @@
         <v>11</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -825,10 +837,10 @@
         <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -836,10 +848,10 @@
         <v>13</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -847,10 +859,10 @@
         <v>14</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -858,10 +870,10 @@
         <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -869,10 +881,10 @@
         <v>16</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -880,10 +892,10 @@
         <v>17</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -891,10 +903,10 @@
         <v>18</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" t="s">
         <v>35</v>
-      </c>
-      <c r="C22" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -902,10 +914,10 @@
         <v>19</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -913,10 +925,10 @@
         <v>20</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -924,10 +936,10 @@
         <v>21</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -935,10 +947,10 @@
         <v>22</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -946,10 +958,10 @@
         <v>23</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C27" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -957,10 +969,10 @@
         <v>24</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -968,10 +980,10 @@
         <v>25</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C29" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -979,10 +991,10 @@
         <v>26</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C30" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -990,10 +1002,10 @@
         <v>27</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C31" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -1001,10 +1013,10 @@
         <v>28</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>54</v>
+        <v>93</v>
       </c>
       <c r="C32" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -1012,10 +1024,10 @@
         <v>29</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="C33" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -1023,10 +1035,7 @@
         <v>30</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C34" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -1034,10 +1043,7 @@
         <v>31</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C35" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -1045,10 +1051,10 @@
         <v>32</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C36" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -1056,10 +1062,10 @@
         <v>33</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C37" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -1067,10 +1073,10 @@
         <v>34</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C38" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -1078,10 +1084,10 @@
         <v>35</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C39" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -1089,10 +1095,10 @@
         <v>36</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C40" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -1100,10 +1106,10 @@
         <v>37</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C41" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -1111,10 +1117,10 @@
         <v>38</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C42" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -1122,10 +1128,10 @@
         <v>39</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C43" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -1133,10 +1139,10 @@
         <v>40</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C44" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -1144,10 +1150,10 @@
         <v>41</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C45" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -1155,10 +1161,10 @@
         <v>42</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="C46" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -1166,10 +1172,10 @@
         <v>43</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C47" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -1180,7 +1186,7 @@
         <v>69</v>
       </c>
       <c r="C48" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -1188,10 +1194,10 @@
         <v>45</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C49" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -1199,10 +1205,10 @@
         <v>46</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="C50" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -1210,7 +1216,10 @@
         <v>47</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>81</v>
+        <v>61</v>
+      </c>
+      <c r="C51" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
@@ -1218,10 +1227,10 @@
         <v>48</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="C52" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
@@ -1229,10 +1238,10 @@
         <v>49</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C53" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
@@ -1240,10 +1249,10 @@
         <v>50</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C54" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
@@ -1251,10 +1260,7 @@
         <v>51</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C55" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
@@ -1262,6 +1268,9 @@
         <v>52</v>
       </c>
       <c r="B56" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C56" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1270,7 +1279,10 @@
         <v>53</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
+      </c>
+      <c r="C57" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
@@ -1278,7 +1290,10 @@
         <v>54</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
+      </c>
+      <c r="C58" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
@@ -1286,10 +1301,45 @@
         <v>55</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C59" t="s">
-        <v>91</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>56</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>57</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>58</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>59</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C63" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix ATRG/STRG length/delay register block location
</commit_message>
<xml_diff>
--- a/helix_mtrig_registers.xlsx
+++ b/helix_mtrig_registers.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="98">
   <si>
     <t>Master trigger register map, as of 0.1.3</t>
   </si>
@@ -338,6 +338,9 @@
   </si>
   <si>
     <t>[13:8] current busies, [5:0] busy mask</t>
+  </si>
+  <si>
+    <t>Hex</t>
   </si>
 </sst>
 </file>
@@ -673,672 +676,916 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="str">
+        <f>DEC2HEX(A4)</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="str">
+        <f t="shared" ref="B5:B63" si="0">DEC2HEX(A5)</f>
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>5</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>6</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>7</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>8</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>9</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>10</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>11</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>B</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>12</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>C</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>13</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>D</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>14</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>E</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>15</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>F</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>16</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>17</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>18</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>19</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>20</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>21</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>22</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>23</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>24</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>25</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>26</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>1A</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>27</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C31" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>1B</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>28</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>1C</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>29</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>1D</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>30</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>1E</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>31</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>1F</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>32</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>33</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>34</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>35</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>36</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>37</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>38</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" t="str">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>39</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" t="str">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>40</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" t="str">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>41</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" t="str">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>42</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" t="str">
+        <f t="shared" si="0"/>
+        <v>2A</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>43</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" t="str">
+        <f t="shared" si="0"/>
+        <v>2B</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>44</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" t="str">
+        <f t="shared" si="0"/>
+        <v>2C</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>45</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" t="str">
+        <f t="shared" si="0"/>
+        <v>2D</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>46</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" t="str">
+        <f t="shared" si="0"/>
+        <v>2E</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>47</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" t="str">
+        <f t="shared" si="0"/>
+        <v>2F</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>48</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" t="str">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>49</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" t="str">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>50</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" t="str">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>51</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" t="str">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>52</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" t="str">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>53</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" t="str">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>54</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" t="str">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>55</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" t="str">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>56</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" t="str">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>57</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B61" t="str">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>58</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" t="str">
+        <f t="shared" si="0"/>
+        <v>3A</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>59</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" t="str">
+        <f t="shared" si="0"/>
+        <v>3B</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>